<commit_message>
Added slides for web frameworks
</commit_message>
<xml_diff>
--- a/resources/data/data.xlsx
+++ b/resources/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emewalsh\Desktop\Personal\parallax-stack-overflow-no-framework\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{472CA829-CB27-43D6-A47F-5741951DC6F5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449F32D2-29EB-4474-81D4-DAC575F7D820}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FBDEFA59-7FAE-4DC4-B854-7511491D4AB4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FBDEFA59-7FAE-4DC4-B854-7511491D4AB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Languages" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
   <si>
     <t>Language</t>
   </si>
@@ -210,13 +210,48 @@
   </si>
   <si>
     <t>Erlang</t>
+  </si>
+  <si>
+    <t>This year, we asked about frameworks for the web separately from other frameworks and libraries. jQuery is the most broadly used of these web frameworks, and this year more developers say they use React.js than Angular, a switch from last year.</t>
+  </si>
+  <si>
+    <r>
+      <t>React.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF404041"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF1060E1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Vue.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF404041"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> are both the most loved and most wanted web frameworks by developers, while Drupal and jQuery are most dreaded.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,6 +269,25 @@
     <font>
       <sz val="10"/>
       <color rgb="FF404041"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF404041"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF404041"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF1060E1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -258,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -268,6 +322,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7306F421-F2C6-4CA9-873B-C07ADB86B029}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1077,13 +1140,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F53497D5-F645-404A-8145-241D58E67CB2}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1106,100 +1172,229 @@
       <c r="A2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="1">
-        <v>0.48699999999999999</v>
+      <c r="B2" s="7">
+        <v>48.699999999999996</v>
+      </c>
+      <c r="C2" s="8">
+        <v>45.3</v>
+      </c>
+      <c r="D2" s="9">
+        <f>100 - C2</f>
+        <v>54.7</v>
+      </c>
+      <c r="E2" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="7">
+        <v>31.3</v>
+      </c>
+      <c r="C3" s="8">
+        <v>74.5</v>
+      </c>
+      <c r="D3" s="9">
+        <f>100 - C3</f>
+        <v>25.5</v>
+      </c>
+      <c r="E3" s="8">
+        <v>21.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.313</v>
+        <v>32</v>
+      </c>
+      <c r="B4" s="7">
+        <v>30.7</v>
+      </c>
+      <c r="C4" s="8">
+        <v>57.6</v>
+      </c>
+      <c r="D4" s="9">
+        <f t="shared" ref="D4:D12" si="0">100 - C4</f>
+        <v>42.4</v>
+      </c>
+      <c r="E4" s="8">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="7">
+        <v>26.3</v>
+      </c>
+      <c r="C5" s="8">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="D5" s="9">
+        <f t="shared" si="0"/>
+        <v>35.099999999999994</v>
+      </c>
+      <c r="E5" s="8">
+        <v>3.7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.307</v>
+        <v>34</v>
+      </c>
+      <c r="B6" s="7">
+        <v>19.7</v>
+      </c>
+      <c r="C6" s="8">
+        <v>68.3</v>
+      </c>
+      <c r="D6" s="9">
+        <f t="shared" si="0"/>
+        <v>31.700000000000003</v>
+      </c>
+      <c r="E6" s="8">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="7">
+        <v>16.2</v>
+      </c>
+      <c r="C7" s="8">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="D7" s="9">
+        <f t="shared" si="0"/>
+        <v>34.400000000000006</v>
+      </c>
+      <c r="E7" s="8">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0.26300000000000001</v>
+        <v>36</v>
+      </c>
+      <c r="B8" s="7">
+        <v>15.2</v>
+      </c>
+      <c r="C8" s="8">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="D8" s="9">
+        <f t="shared" si="0"/>
+        <v>26.400000000000006</v>
+      </c>
+      <c r="E8" s="8">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="7">
+        <v>13</v>
+      </c>
+      <c r="C9" s="8">
+        <v>62.1</v>
+      </c>
+      <c r="D9" s="9">
+        <f t="shared" si="0"/>
+        <v>37.9</v>
+      </c>
+      <c r="E9" s="8">
+        <v>7.8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0.19700000000000001</v>
+        <v>38</v>
+      </c>
+      <c r="B10" s="7">
+        <v>12.1</v>
+      </c>
+      <c r="C10" s="8">
+        <v>61.1</v>
+      </c>
+      <c r="D10" s="9">
+        <f t="shared" si="0"/>
+        <v>38.9</v>
+      </c>
+      <c r="E10" s="8">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="7">
+        <v>10.5</v>
+      </c>
+      <c r="C11" s="8">
+        <v>60.1</v>
+      </c>
+      <c r="D11" s="9">
+        <f t="shared" si="0"/>
+        <v>39.9</v>
+      </c>
+      <c r="E11" s="8">
+        <v>3.1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0.16200000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="1">
-        <v>0.152</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="1">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0.121</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="1">
-        <v>0.105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="1">
-        <v>8.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B12" s="7">
+        <v>8.2000000000000011</v>
+      </c>
+      <c r="C12" s="8">
+        <v>57.1</v>
+      </c>
+      <c r="D12" s="9">
+        <f t="shared" si="0"/>
+        <v>42.9</v>
+      </c>
+      <c r="E12" s="8">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="1">
-        <v>3.5000000000000003E-2</v>
+      <c r="B13" s="7">
+        <v>3.5000000000000004</v>
+      </c>
+      <c r="C13" s="8">
+        <v>30.1</v>
+      </c>
+      <c r="D13" s="9">
+        <f>100 - C13</f>
+        <v>69.900000000000006</v>
+      </c>
+      <c r="E13" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="256.2" x14ac:dyDescent="0.3">
+      <c r="B17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>